<commit_message>
Testing radial field scan cuts
</commit_message>
<xml_diff>
--- a/Sheets/ExpectedAEDM.xlsx
+++ b/Sheets/ExpectedAEDM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5BF8E5-1727-C54A-9212-AA87AE65D11F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A5717-0A91-E54C-B952-18C4659A8D08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3640" yWindow="-19420" windowWidth="28040" windowHeight="17040" xr2:uid="{EFBB272C-EAE8-5B40-912F-21F288E205C9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EFBB272C-EAE8-5B40-912F-21F288E205C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="191" formatCode="0.00000000000000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000000000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -175,8 +175,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,25 +491,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA378DCD-9885-FF42-AB49-0A9292DB66AB}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="7" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
@@ -529,7 +530,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -556,7 +557,7 @@
         <v>5.0053726546566542E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -589,8 +590,16 @@
         <f>J4/K4</f>
         <v>0.13</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <f>I4/C19</f>
+        <v>1.6893116653843927E-3</v>
+      </c>
+      <c r="N4">
+        <f>M4*1000</f>
+        <v>1.6893116653843927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -620,7 +629,7 @@
         <v>1.647099806773175</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -628,10 +637,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -642,7 +651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -663,7 +672,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -682,17 +691,17 @@
         <v>0.10063270353449998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
@@ -703,7 +712,7 @@
         <v>1.1659208900000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>